<commit_message>
updating PIT4 features file
</commit_message>
<xml_diff>
--- a/PIT/PIT Next Version Features.xlsx
+++ b/PIT/PIT Next Version Features.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owalsh01\IdeaProjects\paye-employers-documentation\src\main\resources\PIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5157827-4B43-4117-BDE0-A28A227A9BEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8415"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="8415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIT Next Version Features" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'PIT Next Version Features'!$B$1:$J$28</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'PIT Next Version Features'!$B$1:$J$30</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="34">
   <si>
     <t>Issue Reference</t>
   </si>
@@ -99,12 +100,42 @@
   </si>
   <si>
     <t>Cessation Date now returned for the CSV response of an RPN lookup</t>
+  </si>
+  <si>
+    <t>ESEHTWO-941</t>
+  </si>
+  <si>
+    <t>Pay Period added to Payroll Schema</t>
+  </si>
+  <si>
+    <t>This field is manditory for 2020 submissions and will be used by Revenue PAYE services to assist with the accuracy of in-year reconciliations for Employees which are performed to determine if tax credits/rate bands are allocated to best effect.</t>
+  </si>
+  <si>
+    <t>Submission</t>
+  </si>
+  <si>
+    <t>Payroll</t>
+  </si>
+  <si>
+    <t>In Development</t>
+  </si>
+  <si>
+    <t>ESEHTWO-1046</t>
+  </si>
+  <si>
+    <t>RPN Schema updated to make USC fields Mandatory</t>
+  </si>
+  <si>
+    <t>The payForUSCToDate and uscDeducted fields are now mandatory on 2020 RPN responses. If no value is present, zero will be returned.</t>
+  </si>
+  <si>
+    <t>Expected 10/10/2019</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -184,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -237,6 +268,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -620,7 +654,7 @@
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="Times New Roman"/>
             </a:rPr>
-            <a:t>02/09/2019</a:t>
+            <a:t>07/10/2019</a:t>
           </a:r>
           <a:endParaRPr lang="en-IE" sz="1100">
             <a:effectLst/>
@@ -931,14 +965,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1353,13 +1387,59 @@
       </c>
       <c r="J28" s="4"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B29" s="13"/>
-      <c r="H29" s="7"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B30" s="13"/>
-      <c r="H30" s="7"/>
+    <row r="29" spans="1:17" ht="90" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I29" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="1:17" ht="45" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I30" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="J30" s="4"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B31" s="13"/>

</xml_diff>